<commit_message>
fix error in AF3 prediction data
</commit_message>
<xml_diff>
--- a/10_alphafold_analysis/AF3_new_test_data.xlsx
+++ b/10_alphafold_analysis/AF3_new_test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ffd16e31ab085cd5/Krasevia_Lab/Manuscripts/2025/MAMP_Prediction/Figures/Figure4/Figure4ef/AF3_new_test_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="983" documentId="8_{FEF538B2-1593-C448-8EC7-3EDDBF7DFDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7AEE645D-3FC0-624F-9D62-0BA2990C5B1E}"/>
+  <xr:revisionPtr revIDLastSave="1015" documentId="8_{FEF538B2-1593-C448-8EC7-3EDDBF7DFDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14CF0E03-CFB0-244D-B9C5-286BB0086976}"/>
   <bookViews>
-    <workbookView xWindow="6880" yWindow="500" windowWidth="26720" windowHeight="19540" activeTab="1" xr2:uid="{ADA0C2E5-2BE5-924D-A168-951FD144A553}"/>
+    <workbookView xWindow="6880" yWindow="500" windowWidth="26720" windowHeight="19540" xr2:uid="{ADA0C2E5-2BE5-924D-A168-951FD144A553}"/>
   </bookViews>
   <sheets>
     <sheet name="AF3" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2484" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2548" uniqueCount="288">
   <si>
     <t>Plant species</t>
   </si>
@@ -898,6 +898,9 @@
   </si>
   <si>
     <t>VC130</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -992,7 +995,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1024,9 +1027,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1344,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6308E080-5317-D041-B6EF-5DC04FFC195D}">
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="F139" sqref="F139"/>
+    <sheetView tabSelected="1" topLeftCell="F95" workbookViewId="0">
+      <selection activeCell="L130" sqref="L130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4169,6 +4169,9 @@
       <c r="K74" s="6">
         <v>0.41</v>
       </c>
+      <c r="L74" s="7" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="6" t="s">
@@ -4344,7 +4347,7 @@
       <c r="G79" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H79" s="14" t="s">
+      <c r="H79" s="5" t="s">
         <v>88</v>
       </c>
       <c r="I79" s="5" t="s">
@@ -4382,7 +4385,7 @@
       <c r="G80" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="H80" s="14" t="s">
+      <c r="H80" s="5" t="s">
         <v>89</v>
       </c>
       <c r="I80" s="5" t="s">
@@ -4420,7 +4423,7 @@
       <c r="G81" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H81" s="14" t="s">
+      <c r="H81" s="5" t="s">
         <v>90</v>
       </c>
       <c r="I81" s="5" t="s">
@@ -4458,7 +4461,7 @@
       <c r="G82" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="H82" s="14" t="s">
+      <c r="H82" s="5" t="s">
         <v>91</v>
       </c>
       <c r="I82" s="7" t="s">
@@ -4469,6 +4472,9 @@
       </c>
       <c r="K82" s="6">
         <v>0.46</v>
+      </c>
+      <c r="L82" s="7" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
@@ -4493,7 +4499,7 @@
       <c r="G83" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H83" s="14" t="s">
+      <c r="H83" s="5" t="s">
         <v>191</v>
       </c>
       <c r="I83" s="5" t="s">
@@ -4531,7 +4537,7 @@
       <c r="G84" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H84" s="14" t="s">
+      <c r="H84" s="5" t="s">
         <v>92</v>
       </c>
       <c r="I84" s="5" t="s">
@@ -4569,7 +4575,7 @@
       <c r="G85" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H85" s="14" t="s">
+      <c r="H85" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I85" s="5" t="s">
@@ -4607,7 +4613,7 @@
       <c r="G86" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H86" s="14" t="s">
+      <c r="H86" s="5" t="s">
         <v>94</v>
       </c>
       <c r="I86" s="5" t="s">
@@ -4645,7 +4651,7 @@
       <c r="G87" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H87" s="14" t="s">
+      <c r="H87" s="5" t="s">
         <v>95</v>
       </c>
       <c r="I87" s="5" t="s">
@@ -4683,7 +4689,7 @@
       <c r="G88" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H88" s="14" t="s">
+      <c r="H88" s="5" t="s">
         <v>96</v>
       </c>
       <c r="I88" s="5" t="s">
@@ -4721,7 +4727,7 @@
       <c r="G89" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H89" s="14" t="s">
+      <c r="H89" s="5" t="s">
         <v>97</v>
       </c>
       <c r="I89" s="5" t="s">
@@ -4759,7 +4765,7 @@
       <c r="G90" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H90" s="14" t="s">
+      <c r="H90" s="5" t="s">
         <v>98</v>
       </c>
       <c r="I90" s="5" t="s">
@@ -4797,7 +4803,7 @@
       <c r="G91" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H91" s="14" t="s">
+      <c r="H91" s="5" t="s">
         <v>99</v>
       </c>
       <c r="I91" s="5" t="s">
@@ -4835,7 +4841,7 @@
       <c r="G92" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H92" s="14" t="s">
+      <c r="H92" s="5" t="s">
         <v>100</v>
       </c>
       <c r="I92" s="7" t="s">
@@ -4846,6 +4852,9 @@
       </c>
       <c r="K92" s="6">
         <v>0.44</v>
+      </c>
+      <c r="L92" s="7" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.2">
@@ -4870,7 +4879,7 @@
       <c r="G93" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="H93" s="14" t="s">
+      <c r="H93" s="5" t="s">
         <v>192</v>
       </c>
       <c r="I93" s="5" t="s">
@@ -4882,7 +4891,7 @@
       <c r="K93" s="6">
         <v>0.68</v>
       </c>
-      <c r="L93" t="s">
+      <c r="L93" s="5" t="s">
         <v>189</v>
       </c>
     </row>
@@ -4908,7 +4917,7 @@
       <c r="G94" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H94" s="14" t="s">
+      <c r="H94" s="5" t="s">
         <v>101</v>
       </c>
       <c r="I94" s="5" t="s">
@@ -4946,7 +4955,7 @@
       <c r="G95" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H95" s="14" t="s">
+      <c r="H95" s="5" t="s">
         <v>102</v>
       </c>
       <c r="I95" s="5" t="s">
@@ -4984,7 +4993,7 @@
       <c r="G96" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H96" s="14" t="s">
+      <c r="H96" s="5" t="s">
         <v>103</v>
       </c>
       <c r="I96" s="5" t="s">
@@ -5022,7 +5031,7 @@
       <c r="G97" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H97" s="14" t="s">
+      <c r="H97" s="5" t="s">
         <v>104</v>
       </c>
       <c r="I97" s="5" t="s">
@@ -5060,7 +5069,7 @@
       <c r="G98" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H98" s="14" t="s">
+      <c r="H98" s="5" t="s">
         <v>105</v>
       </c>
       <c r="I98" s="5" t="s">
@@ -5073,7 +5082,7 @@
         <v>0.48</v>
       </c>
       <c r="L98" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.2">
@@ -5098,7 +5107,7 @@
       <c r="G99" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H99" s="14" t="s">
+      <c r="H99" s="5" t="s">
         <v>106</v>
       </c>
       <c r="I99" s="5" t="s">
@@ -5136,7 +5145,7 @@
       <c r="G100" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H100" s="14" t="s">
+      <c r="H100" s="5" t="s">
         <v>107</v>
       </c>
       <c r="I100" s="5" t="s">
@@ -5174,7 +5183,7 @@
       <c r="G101" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H101" s="14" t="s">
+      <c r="H101" s="5" t="s">
         <v>108</v>
       </c>
       <c r="I101" s="7" t="s">
@@ -5185,6 +5194,9 @@
       </c>
       <c r="K101" s="6">
         <v>0.76</v>
+      </c>
+      <c r="L101" s="7" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.2">
@@ -5209,7 +5221,7 @@
       <c r="G102" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H102" s="14" t="s">
+      <c r="H102" s="5" t="s">
         <v>109</v>
       </c>
       <c r="I102" s="5" t="s">
@@ -5247,7 +5259,7 @@
       <c r="G103" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H103" s="14" t="s">
+      <c r="H103" s="5" t="s">
         <v>110</v>
       </c>
       <c r="I103" s="5" t="s">
@@ -5285,7 +5297,7 @@
       <c r="G104" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="H104" s="14" t="s">
+      <c r="H104" s="5" t="s">
         <v>193</v>
       </c>
       <c r="I104" s="5" t="s">
@@ -5323,7 +5335,7 @@
       <c r="G105" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H105" s="14" t="s">
+      <c r="H105" s="5" t="s">
         <v>111</v>
       </c>
       <c r="I105" s="5" t="s">
@@ -5361,7 +5373,7 @@
       <c r="G106" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="H106" s="14" t="s">
+      <c r="H106" s="5" t="s">
         <v>194</v>
       </c>
       <c r="I106" s="7" t="s">
@@ -5372,6 +5384,9 @@
       </c>
       <c r="K106" s="6">
         <v>0.52</v>
+      </c>
+      <c r="L106" s="7" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.2">
@@ -5396,7 +5411,7 @@
       <c r="G107" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="H107" s="14" t="s">
+      <c r="H107" s="5" t="s">
         <v>112</v>
       </c>
       <c r="I107" s="7" t="s">
@@ -5407,6 +5422,9 @@
       </c>
       <c r="K107" s="6">
         <v>0.7</v>
+      </c>
+      <c r="L107" s="7" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="108" spans="1:12" x14ac:dyDescent="0.2">
@@ -5431,7 +5449,7 @@
       <c r="G108" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="H108" s="14" t="s">
+      <c r="H108" s="5" t="s">
         <v>267</v>
       </c>
       <c r="I108" s="5" t="s">
@@ -5469,7 +5487,7 @@
       <c r="G109" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H109" s="14" t="s">
+      <c r="H109" s="5" t="s">
         <v>113</v>
       </c>
       <c r="I109" s="5" t="s">
@@ -5507,7 +5525,7 @@
       <c r="G110" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H110" s="14" t="s">
+      <c r="H110" s="5" t="s">
         <v>114</v>
       </c>
       <c r="I110" s="5" t="s">
@@ -6089,6 +6107,9 @@
       <c r="K125" s="6">
         <v>0.49</v>
       </c>
+      <c r="L125" s="7" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="6" t="s">
@@ -6124,6 +6145,9 @@
       <c r="K126" s="6">
         <v>0.56999999999999995</v>
       </c>
+      <c r="L126" s="7" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="127" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A127" s="6" t="s">
@@ -6197,6 +6221,9 @@
       <c r="K128" s="6">
         <v>0.45</v>
       </c>
+      <c r="L128" s="7" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A129" s="6" t="s">
@@ -6269,6 +6296,9 @@
       </c>
       <c r="K130" s="6">
         <v>0.39</v>
+      </c>
+      <c r="L130" s="7" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="131" spans="1:12" x14ac:dyDescent="0.2">
@@ -6320,8 +6350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0BFFA9-DF9D-FC4F-B7CC-94C967530FE3}">
   <dimension ref="A1:L131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E108" workbookViewId="0">
-      <selection activeCell="I131" sqref="I1:I1048576"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6409,7 +6439,9 @@
       <c r="K2" s="6">
         <v>0.44409999999999999</v>
       </c>
-      <c r="L2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
@@ -6445,7 +6477,9 @@
       <c r="K3" s="6">
         <v>0.45029999999999998</v>
       </c>
-      <c r="L3" s="5"/>
+      <c r="L3" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
@@ -6481,7 +6515,9 @@
       <c r="K4" s="6">
         <v>0.43390000000000001</v>
       </c>
-      <c r="L4" s="5"/>
+      <c r="L4" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
@@ -6517,7 +6553,9 @@
       <c r="K5" s="6">
         <v>0.42170000000000002</v>
       </c>
-      <c r="L5" s="5"/>
+      <c r="L5" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
@@ -6553,7 +6591,9 @@
       <c r="K6" s="6">
         <v>0.47420000000000001</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
@@ -6589,7 +6629,9 @@
       <c r="K7" s="6">
         <v>0.4118</v>
       </c>
-      <c r="L7" s="5"/>
+      <c r="L7" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -6625,7 +6667,9 @@
       <c r="K8" s="6">
         <v>0.4219</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
@@ -6661,7 +6705,9 @@
       <c r="K9" s="6">
         <v>0.47020000000000001</v>
       </c>
-      <c r="L9" s="5"/>
+      <c r="L9" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
@@ -6697,7 +6743,9 @@
       <c r="K10" s="6">
         <v>0.40250000000000002</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
@@ -6733,7 +6781,9 @@
       <c r="K11" s="6">
         <v>0.39100000000000001</v>
       </c>
-      <c r="L11" s="5"/>
+      <c r="L11" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
@@ -6769,7 +6819,9 @@
       <c r="K12" s="6">
         <v>0.43180000000000002</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
@@ -6805,7 +6857,9 @@
       <c r="K13" s="6">
         <v>0.42849999999999999</v>
       </c>
-      <c r="L13" s="5"/>
+      <c r="L13" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
@@ -6841,7 +6895,9 @@
       <c r="K14" s="6">
         <v>0.41049999999999998</v>
       </c>
-      <c r="L14" s="5"/>
+      <c r="L14" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
@@ -6877,7 +6933,9 @@
       <c r="K15" s="6">
         <v>0.39729999999999999</v>
       </c>
-      <c r="L15" s="5"/>
+      <c r="L15" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
@@ -6913,7 +6971,9 @@
       <c r="K16" s="6">
         <v>0.34620000000000001</v>
       </c>
-      <c r="L16" s="5"/>
+      <c r="L16" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
@@ -6949,7 +7009,9 @@
       <c r="K17" s="6">
         <v>0.3926</v>
       </c>
-      <c r="L17" s="5"/>
+      <c r="L17" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
@@ -6985,7 +7047,9 @@
       <c r="K18" s="6">
         <v>0.3649</v>
       </c>
-      <c r="L18" s="5"/>
+      <c r="L18" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
@@ -7021,7 +7085,9 @@
       <c r="K19" s="6">
         <v>0.4783</v>
       </c>
-      <c r="L19" s="5"/>
+      <c r="L19" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
@@ -7057,7 +7123,9 @@
       <c r="K20" s="6">
         <v>0.42470000000000002</v>
       </c>
-      <c r="L20" s="5"/>
+      <c r="L20" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
@@ -7093,7 +7161,9 @@
       <c r="K21" s="6">
         <v>0.4531</v>
       </c>
-      <c r="L21" s="5"/>
+      <c r="L21" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
@@ -7129,7 +7199,9 @@
       <c r="K22" s="6">
         <v>0.38119999999999998</v>
       </c>
-      <c r="L22" s="5"/>
+      <c r="L22" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
@@ -7165,7 +7237,9 @@
       <c r="K23" s="6">
         <v>0.39760000000000001</v>
       </c>
-      <c r="L23" s="5"/>
+      <c r="L23" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
@@ -7201,7 +7275,9 @@
       <c r="K24" s="6">
         <v>0.4032</v>
       </c>
-      <c r="L24" s="5"/>
+      <c r="L24" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
@@ -7237,7 +7313,9 @@
       <c r="K25" s="6">
         <v>0.38290000000000002</v>
       </c>
-      <c r="L25" s="5"/>
+      <c r="L25" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
@@ -7273,7 +7351,9 @@
       <c r="K26" s="6">
         <v>0.43669999999999998</v>
       </c>
-      <c r="L26" s="5"/>
+      <c r="L26" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
@@ -7309,7 +7389,9 @@
       <c r="K27" s="6">
         <v>0.38080000000000003</v>
       </c>
-      <c r="L27" s="5"/>
+      <c r="L27" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
@@ -7345,7 +7427,9 @@
       <c r="K28" s="6">
         <v>0.38750000000000001</v>
       </c>
-      <c r="L28" s="5"/>
+      <c r="L28" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
@@ -7381,7 +7465,9 @@
       <c r="K29" s="6">
         <v>0.38740000000000002</v>
       </c>
-      <c r="L29" s="5"/>
+      <c r="L29" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
@@ -7417,7 +7503,9 @@
       <c r="K30" s="6">
         <v>0.3947</v>
       </c>
-      <c r="L30" s="5"/>
+      <c r="L30" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
@@ -7453,7 +7541,9 @@
       <c r="K31" s="6">
         <v>0.44330000000000003</v>
       </c>
-      <c r="L31" s="5"/>
+      <c r="L31" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
@@ -7489,7 +7579,9 @@
       <c r="K32" s="6">
         <v>0.41589999999999999</v>
       </c>
-      <c r="L32" s="5"/>
+      <c r="L32" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
@@ -7525,7 +7617,9 @@
       <c r="K33" s="6">
         <v>0.41660000000000003</v>
       </c>
-      <c r="L33" s="5"/>
+      <c r="L33" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
@@ -7561,7 +7655,9 @@
       <c r="K34" s="6">
         <v>0.46629999999999999</v>
       </c>
-      <c r="L34" s="5"/>
+      <c r="L34" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
@@ -7597,7 +7693,9 @@
       <c r="K35" s="6">
         <v>0.43519999999999998</v>
       </c>
-      <c r="L35" s="5"/>
+      <c r="L35" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
@@ -7633,7 +7731,9 @@
       <c r="K36" s="13">
         <v>0.42649999999999999</v>
       </c>
-      <c r="L36" s="5"/>
+      <c r="L36" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
@@ -7669,7 +7769,9 @@
       <c r="K37" s="6">
         <v>0.37769999999999998</v>
       </c>
-      <c r="L37" s="5"/>
+      <c r="L37" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
@@ -7705,7 +7807,9 @@
       <c r="K38" s="6">
         <v>0.3715</v>
       </c>
-      <c r="L38" s="5"/>
+      <c r="L38" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
@@ -7741,7 +7845,9 @@
       <c r="K39" s="6">
         <v>0.41010000000000002</v>
       </c>
-      <c r="L39" s="5"/>
+      <c r="L39" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
@@ -7777,7 +7883,9 @@
       <c r="K40" s="6">
         <v>0.31080000000000002</v>
       </c>
-      <c r="L40" s="5"/>
+      <c r="L40" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
@@ -7813,7 +7921,9 @@
       <c r="K41" s="6">
         <v>0.36030000000000001</v>
       </c>
-      <c r="L41" s="5"/>
+      <c r="L41" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
@@ -7849,7 +7959,9 @@
       <c r="K42" s="6">
         <v>0.36520000000000002</v>
       </c>
-      <c r="L42" s="5"/>
+      <c r="L42" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
@@ -7885,7 +7997,9 @@
       <c r="K43" s="6">
         <v>0.4304</v>
       </c>
-      <c r="L43" s="5"/>
+      <c r="L43" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
@@ -7921,7 +8035,9 @@
       <c r="K44" s="6">
         <v>0.37769999999999998</v>
       </c>
-      <c r="L44" s="5"/>
+      <c r="L44" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
@@ -7957,7 +8073,9 @@
       <c r="K45" s="6">
         <v>0.40339999999999998</v>
       </c>
-      <c r="L45" s="5"/>
+      <c r="L45" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
@@ -7993,7 +8111,9 @@
       <c r="K46" s="6">
         <v>0.44379999999999997</v>
       </c>
-      <c r="L46" s="5"/>
+      <c r="L46" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
@@ -8029,7 +8149,9 @@
       <c r="K47" s="6">
         <v>0.38879999999999998</v>
       </c>
-      <c r="L47" s="5"/>
+      <c r="L47" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
@@ -8065,7 +8187,9 @@
       <c r="K48" s="6">
         <v>0.37240000000000001</v>
       </c>
-      <c r="L48" s="5"/>
+      <c r="L48" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
@@ -8101,7 +8225,9 @@
       <c r="K49" s="6">
         <v>0.38890000000000002</v>
       </c>
-      <c r="L49" s="5"/>
+      <c r="L49" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
@@ -8137,7 +8263,9 @@
       <c r="K50" s="6">
         <v>0.3679</v>
       </c>
-      <c r="L50" s="5"/>
+      <c r="L50" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
@@ -8173,7 +8301,9 @@
       <c r="K51" s="6">
         <v>0.39739999999999998</v>
       </c>
-      <c r="L51" s="5"/>
+      <c r="L51" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
@@ -8209,7 +8339,9 @@
       <c r="K52" s="6">
         <v>0.3876</v>
       </c>
-      <c r="L52" s="5"/>
+      <c r="L52" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
@@ -8245,7 +8377,9 @@
       <c r="K53" s="6">
         <v>0.3891</v>
       </c>
-      <c r="L53" s="5"/>
+      <c r="L53" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
@@ -8281,7 +8415,9 @@
       <c r="K54" s="6">
         <v>0.40510000000000002</v>
       </c>
-      <c r="L54" s="5"/>
+      <c r="L54" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
@@ -8317,7 +8453,9 @@
       <c r="K55" s="6">
         <v>0.29549999999999998</v>
       </c>
-      <c r="L55" s="5"/>
+      <c r="L55" s="5" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
@@ -9311,7 +9449,7 @@
       <c r="G83" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="H83" s="14" t="s">
+      <c r="H83" s="5" t="s">
         <v>191</v>
       </c>
       <c r="I83" s="5" t="s">
@@ -9347,7 +9485,7 @@
       <c r="G84" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="H84" s="14" t="s">
+      <c r="H84" s="5" t="s">
         <v>92</v>
       </c>
       <c r="I84" s="5" t="s">
@@ -9383,7 +9521,7 @@
       <c r="G85" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H85" s="14" t="s">
+      <c r="H85" s="5" t="s">
         <v>93</v>
       </c>
       <c r="I85" s="5" t="s">
@@ -9419,7 +9557,7 @@
       <c r="G86" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="H86" s="14" t="s">
+      <c r="H86" s="5" t="s">
         <v>94</v>
       </c>
       <c r="I86" s="5" t="s">
@@ -9455,7 +9593,7 @@
       <c r="G87" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="H87" s="14" t="s">
+      <c r="H87" s="5" t="s">
         <v>95</v>
       </c>
       <c r="I87" s="5" t="s">
@@ -9491,7 +9629,7 @@
       <c r="G88" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="H88" s="14" t="s">
+      <c r="H88" s="5" t="s">
         <v>96</v>
       </c>
       <c r="I88" s="5" t="s">
@@ -9527,7 +9665,7 @@
       <c r="G89" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="H89" s="14" t="s">
+      <c r="H89" s="5" t="s">
         <v>97</v>
       </c>
       <c r="I89" s="5" t="s">
@@ -9563,7 +9701,7 @@
       <c r="G90" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H90" s="14" t="s">
+      <c r="H90" s="5" t="s">
         <v>98</v>
       </c>
       <c r="I90" s="5" t="s">
@@ -9599,7 +9737,7 @@
       <c r="G91" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H91" s="14" t="s">
+      <c r="H91" s="5" t="s">
         <v>99</v>
       </c>
       <c r="I91" s="5" t="s">
@@ -9635,7 +9773,7 @@
       <c r="G92" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="H92" s="14" t="s">
+      <c r="H92" s="5" t="s">
         <v>100</v>
       </c>
       <c r="I92" s="7" t="s">
@@ -9670,7 +9808,7 @@
       <c r="G93" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="H93" s="14" t="s">
+      <c r="H93" s="5" t="s">
         <v>192</v>
       </c>
       <c r="I93" s="5" t="s">
@@ -9705,7 +9843,7 @@
       <c r="G94" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H94" s="14" t="s">
+      <c r="H94" s="5" t="s">
         <v>101</v>
       </c>
       <c r="I94" s="5" t="s">
@@ -9741,7 +9879,7 @@
       <c r="G95" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="H95" s="14" t="s">
+      <c r="H95" s="5" t="s">
         <v>102</v>
       </c>
       <c r="I95" s="5" t="s">
@@ -9777,7 +9915,7 @@
       <c r="G96" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="H96" s="14" t="s">
+      <c r="H96" s="5" t="s">
         <v>103</v>
       </c>
       <c r="I96" s="5" t="s">
@@ -9813,7 +9951,7 @@
       <c r="G97" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H97" s="14" t="s">
+      <c r="H97" s="5" t="s">
         <v>104</v>
       </c>
       <c r="I97" s="5" t="s">
@@ -9849,7 +9987,7 @@
       <c r="G98" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="H98" s="14" t="s">
+      <c r="H98" s="5" t="s">
         <v>105</v>
       </c>
       <c r="I98" s="5" t="s">
@@ -9885,7 +10023,7 @@
       <c r="G99" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="H99" s="14" t="s">
+      <c r="H99" s="5" t="s">
         <v>106</v>
       </c>
       <c r="I99" s="5" t="s">
@@ -9921,7 +10059,7 @@
       <c r="G100" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="H100" s="14" t="s">
+      <c r="H100" s="5" t="s">
         <v>107</v>
       </c>
       <c r="I100" s="5" t="s">
@@ -9957,7 +10095,7 @@
       <c r="G101" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H101" s="14" t="s">
+      <c r="H101" s="5" t="s">
         <v>108</v>
       </c>
       <c r="I101" s="7" t="s">
@@ -9992,7 +10130,7 @@
       <c r="G102" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="H102" s="14" t="s">
+      <c r="H102" s="5" t="s">
         <v>109</v>
       </c>
       <c r="I102" s="5" t="s">
@@ -10028,7 +10166,7 @@
       <c r="G103" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="H103" s="14" t="s">
+      <c r="H103" s="5" t="s">
         <v>110</v>
       </c>
       <c r="I103" s="5" t="s">
@@ -10064,7 +10202,7 @@
       <c r="G104" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="H104" s="14" t="s">
+      <c r="H104" s="5" t="s">
         <v>193</v>
       </c>
       <c r="I104" s="5" t="s">
@@ -10100,7 +10238,7 @@
       <c r="G105" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="H105" s="14" t="s">
+      <c r="H105" s="5" t="s">
         <v>111</v>
       </c>
       <c r="I105" s="5" t="s">
@@ -10136,7 +10274,7 @@
       <c r="G106" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="H106" s="14" t="s">
+      <c r="H106" s="5" t="s">
         <v>194</v>
       </c>
       <c r="I106" s="7" t="s">

</xml_diff>